<commit_message>
Replace blancocg from 2.0.2 to 2.0.3 to adapt PHP namespace.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoRestPhpArraySample.xlsx
+++ b/meta/api/BlancoRestPhpArraySample.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haino/Desktop/blancoRestPhp/meta/api/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestPhp/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7760" yWindow="1520" windowWidth="24240" windowHeight="13700" tabRatio="860"/>
+    <workbookView xWindow="4560" yWindow="1520" windowWidth="24240" windowHeight="13700" tabRatio="860" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="163">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -1712,10 +1712,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>BlancoRestPhp</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>blancoRestPhpのサンプルAPIの要求電文です。</t>
     <rPh sb="22" eb="24">
       <t>ヨウキュウ</t>
@@ -1734,10 +1730,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>BlancoRestPhp</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>blanco.sample.restphp</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -1955,6 +1947,10 @@
       <t>オウトウデンブン</t>
     </rPh>
     <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>blanco\RestPhp</t>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
@@ -2617,6 +2613,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2654,7 +2651,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -3195,8 +3191,8 @@
   </sheetPr>
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3248,7 +3244,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C6" s="26"/>
     </row>
@@ -3263,26 +3259,26 @@
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="120" t="s">
-        <v>162</v>
+      <c r="A8" s="107" t="s">
+        <v>160</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C8" s="26"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="120" t="s">
-        <v>163</v>
+      <c r="A9" s="107" t="s">
+        <v>161</v>
       </c>
       <c r="B9" s="55" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C9" s="26"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B10" s="89"/>
       <c r="C10" s="26"/>
@@ -3292,7 +3288,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C11" s="26"/>
     </row>
@@ -3301,17 +3297,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
       <c r="C12" s="58"/>
       <c r="D12" s="58"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C13" s="58"/>
       <c r="D13" s="58"/>
@@ -3321,7 +3317,7 @@
         <v>27</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C14" s="58"/>
       <c r="D14" s="58"/>
@@ -3342,11 +3338,11 @@
       <c r="A17" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="107" t="s">
+      <c r="B17" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="108"/>
-      <c r="D17" s="109"/>
+      <c r="C17" s="109"/>
+      <c r="D17" s="110"/>
       <c r="E17" s="28" t="s">
         <v>75</v>
       </c>
@@ -3559,7 +3555,7 @@
   <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3596,7 +3592,7 @@
         <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
@@ -3626,7 +3622,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="56" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="58"/>
@@ -3639,7 +3635,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="58"/>
@@ -3665,11 +3661,11 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9" s="60" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="56" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="58"/>
@@ -3681,7 +3677,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="56" t="s">
-        <v>108</v>
+        <v>162</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="58"/>
@@ -3689,11 +3685,11 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="56" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="58"/>
@@ -3729,50 +3725,50 @@
       <c r="R14" s="38"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="110" t="s">
+      <c r="B15" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="112" t="s">
+      <c r="C15" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="110" t="s">
+      <c r="D15" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="110" t="s">
-        <v>149</v>
-      </c>
-      <c r="F15" s="110" t="s">
+      <c r="E15" s="111" t="s">
+        <v>147</v>
+      </c>
+      <c r="F15" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="110" t="s">
-        <v>117</v>
-      </c>
-      <c r="H15" s="113" t="s">
+      <c r="G15" s="111" t="s">
+        <v>115</v>
+      </c>
+      <c r="H15" s="114" t="s">
         <v>79</v>
       </c>
-      <c r="I15" s="114"/>
-      <c r="J15" s="113" t="s">
+      <c r="I15" s="115"/>
+      <c r="J15" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="114"/>
+      <c r="K15" s="115"/>
       <c r="L15" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="M15" s="110" t="s">
+      <c r="M15" s="111" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A16" s="111"/>
-      <c r="B16" s="111"/>
-      <c r="C16" s="111"/>
-      <c r="D16" s="111"/>
-      <c r="E16" s="111"/>
-      <c r="F16" s="111"/>
-      <c r="G16" s="111"/>
+      <c r="A16" s="112"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="112"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="112"/>
+      <c r="G16" s="112"/>
       <c r="H16" s="28" t="s">
         <v>83</v>
       </c>
@@ -3788,27 +3784,27 @@
       <c r="L16" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="M16" s="111"/>
+      <c r="M16" s="112"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" s="7">
         <v>1</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>101</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="88" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H17" s="22">
         <v>0</v>
@@ -3826,14 +3822,14 @@
         <v>2</v>
       </c>
       <c r="B18" s="99" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C18" s="77"/>
       <c r="D18" s="100" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E18" s="100" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F18" s="101"/>
       <c r="G18" s="100"/>
@@ -3843,7 +3839,7 @@
       <c r="K18" s="102"/>
       <c r="L18" s="102"/>
       <c r="M18" s="79" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.15">
@@ -3851,13 +3847,13 @@
         <v>3</v>
       </c>
       <c r="B19" s="106" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>158</v>
-      </c>
       <c r="D19" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="90"/>
@@ -3874,13 +3870,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>159</v>
-      </c>
       <c r="D20" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="90"/>
@@ -3897,13 +3893,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E21" s="24"/>
       <c r="F21" s="90"/>
@@ -4161,8 +4157,8 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4227,7 +4223,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="55" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D6" s="34"/>
       <c r="G6" s="26"/>
@@ -4238,7 +4234,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="56" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D7" s="34"/>
       <c r="G7" s="58"/>
@@ -4260,11 +4256,11 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="60" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B9" s="62"/>
       <c r="C9" s="97" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D9" s="98"/>
     </row>
@@ -4274,17 +4270,17 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="56" t="s">
-        <v>108</v>
+        <v>162</v>
       </c>
       <c r="D10" s="34"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="56" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D11" s="34"/>
     </row>
@@ -4296,7 +4292,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" s="60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B14" s="61"/>
       <c r="C14" s="61"/>
@@ -4312,85 +4308,85 @@
       <c r="M14" s="62"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="119" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="119" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="64" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="118" t="s">
+      <c r="D15" s="119" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="119" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" s="119" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="119" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="116" t="s">
+        <v>121</v>
+      </c>
+      <c r="I15" s="117"/>
+      <c r="J15" s="118" t="s">
+        <v>122</v>
+      </c>
+      <c r="K15" s="117"/>
+      <c r="L15" s="63" t="s">
+        <v>123</v>
+      </c>
+      <c r="M15" s="119" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A16" s="120"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="64" t="s">
-        <v>121</v>
-      </c>
-      <c r="D15" s="118" t="s">
-        <v>113</v>
-      </c>
-      <c r="E15" s="118" t="s">
-        <v>148</v>
-      </c>
-      <c r="F15" s="118" t="s">
-        <v>135</v>
-      </c>
-      <c r="G15" s="118" t="s">
-        <v>134</v>
-      </c>
-      <c r="H15" s="115" t="s">
-        <v>123</v>
-      </c>
-      <c r="I15" s="116"/>
-      <c r="J15" s="117" t="s">
-        <v>124</v>
-      </c>
-      <c r="K15" s="116"/>
-      <c r="L15" s="63" t="s">
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="M15" s="118" t="s">
+      <c r="I16" s="66" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A16" s="119"/>
-      <c r="B16" s="119"/>
-      <c r="C16" s="65" t="s">
-        <v>122</v>
-      </c>
-      <c r="D16" s="119"/>
-      <c r="E16" s="119"/>
-      <c r="F16" s="119"/>
-      <c r="G16" s="119"/>
-      <c r="H16" s="66" t="s">
+      <c r="J16" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="I16" s="66" t="s">
+      <c r="K16" s="66" t="s">
         <v>128</v>
       </c>
-      <c r="J16" s="66" t="s">
+      <c r="L16" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="K16" s="66" t="s">
-        <v>130</v>
-      </c>
-      <c r="L16" s="67" t="s">
-        <v>131</v>
-      </c>
-      <c r="M16" s="119"/>
+      <c r="M16" s="120"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" s="68">
         <v>1</v>
       </c>
       <c r="B17" s="69" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C17" s="70" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D17" s="71" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E17" s="103"/>
       <c r="F17" s="92" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G17" s="71"/>
       <c r="H17" s="71"/>
@@ -4405,14 +4401,14 @@
         <v>2</v>
       </c>
       <c r="B18" s="69" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C18" s="70"/>
       <c r="D18" s="71" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E18" s="104" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F18" s="92"/>
       <c r="G18" s="71"/>
@@ -5185,7 +5181,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -5230,7 +5226,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B13" s="47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Correnct telegram namespace associations.
* absolute or relative spacification of namespaces should be written in Excel sheets.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoRestPhpArraySample.xlsx
+++ b/meta/api/BlancoRestPhpArraySample.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haino/Desktop/blancoRestPhp/meta/api/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestPhp/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="200" yWindow="900" windowWidth="24240" windowHeight="13700" tabRatio="860"/>
+    <workbookView xWindow="200" yWindow="900" windowWidth="24240" windowHeight="13700" tabRatio="860" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="172">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -1905,10 +1905,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>field@hoge</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>field(hoge)abc</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -1964,10 +1960,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>blanco\sample\valueobject</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>電文処理定義・継承</t>
     <rPh sb="0" eb="2">
       <t>デンブn</t>
@@ -1982,6 +1974,30 @@
     <rPh sb="0" eb="2">
       <t>デンブn</t>
     </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ApiBase</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>blanco.sample.valueobjects</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>\blanco\sample\valueobjects</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>\blanco\restphp\common</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>field@hoge2</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>\blanco\RestPhp</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -2791,43 +2807,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2850,6 +2829,43 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -3390,8 +3406,8 @@
   </sheetPr>
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3459,7 +3475,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="105" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B8" s="55" t="s">
         <v>139</v>
@@ -3468,7 +3484,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="105" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B9" s="55" t="s">
         <v>140</v>
@@ -3496,7 +3512,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C12" s="58"/>
       <c r="D12" s="58"/>
@@ -3527,59 +3543,59 @@
       <c r="C15" s="58"/>
       <c r="D15" s="58"/>
     </row>
-    <row r="16" spans="1:10" s="122" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="119" t="s">
-        <v>166</v>
-      </c>
-      <c r="B16" s="120"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="121"/>
+    <row r="16" spans="1:10" s="109" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="106" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="107"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="108"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" s="122" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="123" t="s">
-        <v>161</v>
-      </c>
-      <c r="B17" s="124"/>
-      <c r="C17" s="125" t="s">
-        <v>137</v>
-      </c>
-      <c r="D17" s="125"/>
-      <c r="E17" s="125"/>
-      <c r="F17" s="126"/>
+    <row r="17" spans="1:10" s="109" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="110" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" s="111"/>
+      <c r="C17" s="112" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" s="112"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="113"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" s="122" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="127" t="s">
+    <row r="18" spans="1:10" s="109" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="114" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" s="115"/>
+      <c r="C18" s="116" t="s">
         <v>162</v>
       </c>
-      <c r="B18" s="128"/>
-      <c r="C18" s="129" t="s">
+      <c r="D18" s="117"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="119"/>
+    </row>
+    <row r="19" spans="1:10" s="109" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="114" t="s">
         <v>163</v>
       </c>
-      <c r="D18" s="130"/>
-      <c r="E18" s="131"/>
-      <c r="F18" s="132"/>
-    </row>
-    <row r="19" spans="1:10" s="122" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="127" t="s">
-        <v>164</v>
-      </c>
-      <c r="B19" s="128"/>
-      <c r="C19" s="129" t="s">
-        <v>165</v>
-      </c>
-      <c r="D19" s="130"/>
-      <c r="E19" s="131"/>
-      <c r="F19" s="132"/>
+      <c r="B19" s="115"/>
+      <c r="C19" s="116" t="s">
+        <v>169</v>
+      </c>
+      <c r="D19" s="117"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="119"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="6"/>
@@ -3597,11 +3613,11 @@
       <c r="A22" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="106" t="s">
+      <c r="B22" s="120" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="107"/>
-      <c r="D22" s="108"/>
+      <c r="C22" s="121"/>
+      <c r="D22" s="122"/>
       <c r="E22" s="28" t="s">
         <v>75</v>
       </c>
@@ -3814,7 +3830,7 @@
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3924,7 +3940,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="56" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="58"/>
@@ -3946,59 +3962,59 @@
       <c r="A11" s="6"/>
       <c r="C11" s="26"/>
     </row>
-    <row r="12" spans="1:11" s="122" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="119" t="s">
-        <v>167</v>
-      </c>
-      <c r="B12" s="120"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="120"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="121"/>
+    <row r="12" spans="1:11" s="109" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="106" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" s="107"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="108"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:11" s="122" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="123" t="s">
-        <v>161</v>
-      </c>
-      <c r="B13" s="124"/>
-      <c r="C13" s="125" t="s">
+    <row r="13" spans="1:11" s="109" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="110" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="111"/>
+      <c r="C13" s="112" t="s">
         <v>137</v>
       </c>
-      <c r="D13" s="125"/>
-      <c r="E13" s="125"/>
-      <c r="F13" s="126"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="113"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:11" s="122" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="127" t="s">
-        <v>162</v>
-      </c>
-      <c r="B14" s="128"/>
-      <c r="C14" s="129" t="s">
+    <row r="14" spans="1:11" s="109" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="114" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="115"/>
+      <c r="C14" s="116" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="117"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="119"/>
+    </row>
+    <row r="15" spans="1:11" s="109" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="114" t="s">
         <v>163</v>
       </c>
-      <c r="D14" s="130"/>
-      <c r="E14" s="131"/>
-      <c r="F14" s="132"/>
-    </row>
-    <row r="15" spans="1:11" s="122" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="127" t="s">
-        <v>164</v>
-      </c>
-      <c r="B15" s="128"/>
-      <c r="C15" s="129" t="s">
-        <v>165</v>
-      </c>
-      <c r="D15" s="130"/>
-      <c r="E15" s="131"/>
-      <c r="F15" s="132"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="116" t="s">
+        <v>168</v>
+      </c>
+      <c r="D15" s="117"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="119"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="6"/>
@@ -4026,50 +4042,50 @@
       <c r="R17" s="38"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A18" s="109" t="s">
+      <c r="A18" s="123" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="109" t="s">
+      <c r="B18" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="111" t="s">
+      <c r="C18" s="125" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="109" t="s">
+      <c r="D18" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="109" t="s">
+      <c r="E18" s="123" t="s">
         <v>145</v>
       </c>
-      <c r="F18" s="109" t="s">
+      <c r="F18" s="123" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="109" t="s">
+      <c r="G18" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="H18" s="112" t="s">
+      <c r="H18" s="126" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="113"/>
-      <c r="J18" s="112" t="s">
+      <c r="I18" s="127"/>
+      <c r="J18" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="113"/>
+      <c r="K18" s="127"/>
       <c r="L18" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="M18" s="109" t="s">
+      <c r="M18" s="123" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A19" s="110"/>
-      <c r="B19" s="110"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="110"/>
-      <c r="G19" s="110"/>
+      <c r="A19" s="124"/>
+      <c r="B19" s="124"/>
+      <c r="C19" s="124"/>
+      <c r="D19" s="124"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="124"/>
       <c r="H19" s="28" t="s">
         <v>83</v>
       </c>
@@ -4085,7 +4101,7 @@
       <c r="L19" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="M19" s="110"/>
+      <c r="M19" s="124"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="7">
@@ -4148,10 +4164,10 @@
         <v>3</v>
       </c>
       <c r="B22" s="104" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>113</v>
@@ -4171,10 +4187,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>113</v>
@@ -4194,10 +4210,10 @@
         <v>5</v>
       </c>
       <c r="B24" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>113</v>
@@ -4428,7 +4444,6 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" display="http://tempuri.org/sample"/>
-    <hyperlink ref="B22" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.11811023622047245"/>
   <pageSetup paperSize="9" scale="63" fitToHeight="0" orientation="landscape"/>
@@ -4458,8 +4473,8 @@
   </sheetPr>
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4561,7 +4576,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="56" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="D9" s="34"/>
     </row>
@@ -4578,59 +4593,59 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="6"/>
     </row>
-    <row r="12" spans="1:11" s="122" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="119" t="s">
-        <v>167</v>
-      </c>
-      <c r="B12" s="120"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="120"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="121"/>
+    <row r="12" spans="1:11" s="109" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="106" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" s="107"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="108"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:11" s="122" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="123" t="s">
-        <v>161</v>
-      </c>
-      <c r="B13" s="124"/>
-      <c r="C13" s="125" t="s">
+    <row r="13" spans="1:11" s="109" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="110" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="111"/>
+      <c r="C13" s="112" t="s">
         <v>137</v>
       </c>
-      <c r="D13" s="125"/>
-      <c r="E13" s="125"/>
-      <c r="F13" s="126"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="113"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:11" s="122" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="127" t="s">
-        <v>162</v>
-      </c>
-      <c r="B14" s="128"/>
-      <c r="C14" s="129" t="s">
+    <row r="14" spans="1:11" s="109" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="114" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="115"/>
+      <c r="C14" s="116" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="117"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="119"/>
+    </row>
+    <row r="15" spans="1:11" s="109" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="114" t="s">
         <v>163</v>
       </c>
-      <c r="D14" s="130"/>
-      <c r="E14" s="131"/>
-      <c r="F14" s="132"/>
-    </row>
-    <row r="15" spans="1:11" s="122" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="127" t="s">
-        <v>164</v>
-      </c>
-      <c r="B15" s="128"/>
-      <c r="C15" s="129" t="s">
-        <v>165</v>
-      </c>
-      <c r="D15" s="130"/>
-      <c r="E15" s="131"/>
-      <c r="F15" s="132"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="116" t="s">
+        <v>168</v>
+      </c>
+      <c r="D15" s="117"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="119"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="6"/>
@@ -4653,52 +4668,52 @@
       <c r="M17" s="62"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A18" s="117" t="s">
+      <c r="A18" s="131" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="117" t="s">
+      <c r="B18" s="131" t="s">
         <v>118</v>
       </c>
       <c r="C18" s="64" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="117" t="s">
+      <c r="D18" s="131" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="117" t="s">
+      <c r="E18" s="131" t="s">
         <v>144</v>
       </c>
-      <c r="F18" s="117" t="s">
+      <c r="F18" s="131" t="s">
         <v>133</v>
       </c>
-      <c r="G18" s="117" t="s">
+      <c r="G18" s="131" t="s">
         <v>132</v>
       </c>
-      <c r="H18" s="114" t="s">
+      <c r="H18" s="128" t="s">
         <v>121</v>
       </c>
-      <c r="I18" s="115"/>
-      <c r="J18" s="116" t="s">
+      <c r="I18" s="129"/>
+      <c r="J18" s="130" t="s">
         <v>122</v>
       </c>
-      <c r="K18" s="115"/>
+      <c r="K18" s="129"/>
       <c r="L18" s="63" t="s">
         <v>123</v>
       </c>
-      <c r="M18" s="117" t="s">
+      <c r="M18" s="131" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A19" s="118"/>
-      <c r="B19" s="118"/>
+      <c r="A19" s="132"/>
+      <c r="B19" s="132"/>
       <c r="C19" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="D19" s="118"/>
-      <c r="E19" s="118"/>
-      <c r="F19" s="118"/>
-      <c r="G19" s="118"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="132"/>
+      <c r="F19" s="132"/>
+      <c r="G19" s="132"/>
       <c r="H19" s="66" t="s">
         <v>125</v>
       </c>
@@ -4714,7 +4729,7 @@
       <c r="L19" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="M19" s="118"/>
+      <c r="M19" s="132"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20" s="68">

</xml_diff>